<commit_message>
Small tweaks to files
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\GitHub\germination_stan\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27729"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11760"/>
+    <workbookView xWindow="100" yWindow="0" windowWidth="25180" windowHeight="15820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
+    <sheet name="meta" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,10 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
-  <si>
-    <t>Fake data assignment</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Variable</t>
   </si>
@@ -116,12 +112,6 @@
     <t>origintempstrat</t>
   </si>
   <si>
-    <t>WITH SPECIES</t>
-  </si>
-  <si>
-    <t>WITHOUT SPECIES</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -146,14 +136,38 @@
     <t xml:space="preserve">species 7 intercept </t>
   </si>
   <si>
-    <t>WITH SPECIES SANS INTERACTIONS</t>
+    <t>Below metadata by Lizzie Wolkovich (EMW):</t>
+  </si>
+  <si>
+    <t>On 3 January 2017:</t>
+  </si>
+  <si>
+    <t>This file was started by Harold Eyster a couple weeks back to trouble-shoot Stan model building with (initially) fake data then real data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It goes through the values given to the model from fake data and reports -- for different Stan models -- what the model returned. </t>
+  </si>
+  <si>
+    <t>WITH SPECIES SANS INTERACTIONS (germdate_sp_no-inter.stan)</t>
+  </si>
+  <si>
+    <t>Fake data assignment (germdate_fakedata.R)</t>
+  </si>
+  <si>
+    <t>WITH SPECIES (germdate_sp.stan)</t>
+  </si>
+  <si>
+    <t>WITHOUT SPECIES (germdate.stan)</t>
+  </si>
+  <si>
+    <t>Red means …</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +192,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,37 +249,41 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -271,8 +305,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -331,7 +370,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -383,7 +422,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -577,7 +616,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -587,19 +626,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V21" sqref="V21"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C8" sqref="B7:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20">
       <c r="C1" s="2" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -607,7 +646,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="4"/>
       <c r="I1" s="3" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -615,7 +654,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P1" s="16"/>
       <c r="Q1" s="16"/>
@@ -623,15 +662,15 @@
       <c r="S1" s="16"/>
       <c r="T1" s="16"/>
     </row>
-    <row r="2" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="5" customFormat="1">
       <c r="A2" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="7">
         <v>2.5000000000000001E-2</v>
@@ -649,7 +688,7 @@
         <v>0.97499999999999998</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J2" s="11">
         <v>2.5000000000000001E-2</v>
@@ -667,7 +706,7 @@
         <v>0.97499999999999998</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P2" s="14">
         <v>2.5000000000000001E-2</v>
@@ -685,9 +724,9 @@
         <v>0.97499999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>0.01</v>
@@ -711,9 +750,9 @@
       <c r="S3" s="16"/>
       <c r="T3" s="16"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>-0.01</v>
@@ -737,9 +776,9 @@
       <c r="S4" s="16"/>
       <c r="T4" s="16"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>0.02</v>
@@ -763,9 +802,9 @@
       <c r="S5" s="16"/>
       <c r="T5" s="16"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2">
         <v>-0.02</v>
@@ -822,9 +861,9 @@
         <v>1.54E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>0.9</v>
@@ -884,9 +923,9 @@
         <v>1.2565999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>0.01</v>
@@ -946,9 +985,9 @@
         <v>2.7300000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <v>1.4E-2</v>
@@ -996,9 +1035,9 @@
         <v>1.6400000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>0.4</v>
@@ -1046,9 +1085,9 @@
         <v>0.61580000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>5.0000000000000001E-3</v>
@@ -1096,7 +1135,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1116,9 +1155,9 @@
       <c r="S12" s="16"/>
       <c r="T12" s="16"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13">
         <v>-7.0000000000000007E-2</v>
@@ -1142,9 +1181,9 @@
       <c r="S13" s="16"/>
       <c r="T13" s="16"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>-0.02</v>
@@ -1168,9 +1207,9 @@
       <c r="S14" s="16"/>
       <c r="T14" s="16"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <v>-0.09</v>
@@ -1194,9 +1233,9 @@
       <c r="S15" s="16"/>
       <c r="T15" s="16"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="2">
         <v>5.0000000000000001E-3</v>
@@ -1241,9 +1280,9 @@
       <c r="S16" s="16"/>
       <c r="T16" s="16"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>-2E-3</v>
@@ -1267,9 +1306,9 @@
       <c r="S17" s="16"/>
       <c r="T17" s="16"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18">
         <v>-1E-3</v>
@@ -1293,9 +1332,9 @@
       <c r="S18" s="16"/>
       <c r="T18" s="16"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19">
         <v>-2.5000000000000001E-3</v>
@@ -1319,9 +1358,9 @@
       <c r="S19" s="16"/>
       <c r="T19" s="16"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="2">
         <v>3.5000000000000003E-2</v>
@@ -1366,9 +1405,9 @@
       <c r="S20" s="16"/>
       <c r="T20" s="16"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21">
         <v>-2.1999999999999999E-2</v>
@@ -1416,9 +1455,9 @@
       <c r="S21" s="16"/>
       <c r="T21" s="16"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22">
         <v>5.0000000000000001E-3</v>
@@ -1442,9 +1481,9 @@
       <c r="S22" s="16"/>
       <c r="T22" s="16"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23">
         <v>1E-3</v>
@@ -1468,9 +1507,9 @@
       <c r="S23" s="16"/>
       <c r="T23" s="16"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24">
         <v>5.0000000000000001E-3</v>
@@ -1494,9 +1533,9 @@
       <c r="S24" s="16"/>
       <c r="T24" s="16"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="2">
         <v>-2.1000000000000001E-2</v>
@@ -1541,9 +1580,9 @@
       <c r="S25" s="16"/>
       <c r="T25" s="16"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26">
         <v>2.1000000000000001E-2</v>
@@ -1579,9 +1618,9 @@
       <c r="S26" s="16"/>
       <c r="T26" s="16"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27">
         <v>2.9999999999999997E-4</v>
@@ -1617,9 +1656,9 @@
       <c r="S27" s="16"/>
       <c r="T27" s="16"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28">
         <v>4.0000000000000002E-4</v>
@@ -1655,9 +1694,9 @@
       <c r="S28" s="16"/>
       <c r="T28" s="16"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29">
         <v>1E-3</v>
@@ -1693,7 +1732,7 @@
       <c r="S29" s="16"/>
       <c r="T29" s="16"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1713,9 +1752,9 @@
       <c r="S30" s="16"/>
       <c r="T30" s="16"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31">
         <v>2.6</v>
@@ -1751,9 +1790,9 @@
       <c r="S31" s="16"/>
       <c r="T31" s="16"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1">
         <v>0.98</v>
@@ -1795,9 +1834,9 @@
         <v>0.42499999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>1.48</v>
@@ -1839,9 +1878,9 @@
         <v>0.53800000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>1.98</v>
@@ -1883,9 +1922,9 @@
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>2.48</v>
@@ -1927,9 +1966,9 @@
         <v>1.528</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>2.98</v>
@@ -1971,9 +2010,9 @@
         <v>1.861</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>3.48</v>
@@ -2015,9 +2054,9 @@
         <v>2.415</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>3.98</v>
@@ -2059,13 +2098,63 @@
         <v>3.012</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
now with rstanarm models
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27729"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\GitHub\germination_stan\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="100" yWindow="0" windowWidth="25180" windowHeight="15820" activeTab="1"/>
+    <workbookView xWindow="105" yWindow="0" windowWidth="25185" windowHeight="15825"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -12,18 +17,18 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Variable</t>
   </si>
@@ -160,13 +165,28 @@
     <t>WITHOUT SPECIES (germdate.stan)</t>
   </si>
   <si>
-    <t>Red means …</t>
+    <t>WITH SPECIES AND INTERACTIONS (rndm intercept, but not slope). Using rstanarm</t>
+  </si>
+  <si>
+    <t>Red means when the model doesn't include the actual value in it's 95% CrI</t>
+  </si>
+  <si>
+    <t>on 12 March 2017:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added in the model run with rstanarm, using species random intercepts, but not random slopes. Included interactions. This model showed no divergent transitions. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes: this model fits quite well, though origindiff is way off. Running a frequentist lmer yields the same wrong result. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why is the intercept not within the set of species intercepts? </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -283,7 +303,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -306,6 +326,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -616,7 +642,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -624,19 +650,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T39"/>
+  <dimension ref="A1:AK39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C8" sqref="B7:C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="U32" sqref="U32:U38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="21" max="26" width="8.85546875" style="3"/>
+    <col min="31" max="31" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C1" s="2" t="s">
         <v>44</v>
       </c>
@@ -660,9 +690,12 @@
       <c r="Q1" s="16"/>
       <c r="R1" s="16"/>
       <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-    </row>
-    <row r="2" spans="1:20" s="5" customFormat="1">
+      <c r="T1" s="23"/>
+      <c r="U1" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -720,11 +753,29 @@
       <c r="S2" s="15">
         <v>0.75</v>
       </c>
-      <c r="T2" s="14">
+      <c r="T2" s="24">
         <v>0.97499999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="U2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" s="11">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="W2" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="X2" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="Y2" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="Z2" s="11">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -748,9 +799,27 @@
       <c r="Q3" s="16"/>
       <c r="R3" s="16"/>
       <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="T3" s="23"/>
+      <c r="U3" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="V3" s="3">
+        <v>-0.02</v>
+      </c>
+      <c r="W3" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="X3" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -774,9 +843,27 @@
       <c r="Q4" s="16"/>
       <c r="R4" s="16"/>
       <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="T4" s="23"/>
+      <c r="U4" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="V4" s="3">
+        <v>-0.05</v>
+      </c>
+      <c r="W4" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="X4" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -800,9 +887,27 @@
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
       <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="T5" s="23"/>
+      <c r="U5" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="X5" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -857,11 +962,11 @@
       <c r="S6" s="16">
         <v>9.9000000000000008E-3</v>
       </c>
-      <c r="T6" s="16">
+      <c r="T6" s="23">
         <v>1.54E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -919,11 +1024,34 @@
       <c r="S7" s="16">
         <v>1.0882000000000001</v>
       </c>
-      <c r="T7" s="16">
+      <c r="T7" s="23">
         <v>1.2565999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="U7" s="17">
+        <v>0.73</v>
+      </c>
+      <c r="V7" s="17">
+        <v>0.69</v>
+      </c>
+      <c r="W7" s="17">
+        <v>0.71</v>
+      </c>
+      <c r="X7" s="17">
+        <v>0.73</v>
+      </c>
+      <c r="Y7" s="17">
+        <v>0.74</v>
+      </c>
+      <c r="Z7" s="17">
+        <v>0.77</v>
+      </c>
+      <c r="AG7" s="21"/>
+      <c r="AH7" s="22"/>
+      <c r="AI7" s="22"/>
+      <c r="AJ7" s="22"/>
+      <c r="AK7" s="21"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -981,11 +1109,29 @@
       <c r="S8" s="16">
         <v>1.8100000000000002E-2</v>
       </c>
-      <c r="T8" s="16">
+      <c r="T8" s="23">
         <v>2.7300000000000001E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="U8" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="V8" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="W8" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="X8" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1031,11 +1177,11 @@
       <c r="S9" s="16">
         <v>7.6E-3</v>
       </c>
-      <c r="T9" s="16">
+      <c r="T9" s="23">
         <v>1.6400000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1081,11 +1227,11 @@
       <c r="S10" s="16">
         <v>0.34939999999999999</v>
       </c>
-      <c r="T10" s="16">
+      <c r="T10" s="23">
         <v>0.61580000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1131,11 +1277,11 @@
       <c r="S11" s="16">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="T11" s="16">
+      <c r="T11" s="23">
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1153,9 +1299,9 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
       <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="T12" s="23"/>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1179,9 +1325,27 @@
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>
       <c r="S13" s="16"/>
-      <c r="T13" s="16"/>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="T13" s="23"/>
+      <c r="U13" s="3">
+        <v>-0.09</v>
+      </c>
+      <c r="V13" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="W13" s="3">
+        <v>-0.11</v>
+      </c>
+      <c r="X13" s="3">
+        <v>-0.09</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1205,9 +1369,27 @@
       <c r="Q14" s="16"/>
       <c r="R14" s="16"/>
       <c r="S14" s="16"/>
-      <c r="T14" s="16"/>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="T14" s="23"/>
+      <c r="U14" s="3">
+        <v>-0.05</v>
+      </c>
+      <c r="V14" s="3">
+        <v>-0.11</v>
+      </c>
+      <c r="W14" s="3">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="X14" s="3">
+        <v>-0.05</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>-0.02</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1231,9 +1413,27 @@
       <c r="Q15" s="16"/>
       <c r="R15" s="16"/>
       <c r="S15" s="16"/>
-      <c r="T15" s="16"/>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="T15" s="23"/>
+      <c r="U15" s="3">
+        <v>-0.13</v>
+      </c>
+      <c r="V15" s="3">
+        <v>-0.19</v>
+      </c>
+      <c r="W15" s="3">
+        <v>-0.15</v>
+      </c>
+      <c r="X15" s="3">
+        <v>-0.12</v>
+      </c>
+      <c r="Y15" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="Z15" s="3">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1278,9 +1478,9 @@
       <c r="Q16" s="16"/>
       <c r="R16" s="16"/>
       <c r="S16" s="16"/>
-      <c r="T16" s="16"/>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="T16" s="23"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1304,9 +1504,27 @@
       <c r="Q17" s="16"/>
       <c r="R17" s="16"/>
       <c r="S17" s="16"/>
-      <c r="T17" s="16"/>
-    </row>
-    <row r="18" spans="1:20">
+      <c r="T17" s="23"/>
+      <c r="U17" s="3">
+        <v>0</v>
+      </c>
+      <c r="V17" s="3">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="W17" s="3">
+        <v>-0.02</v>
+      </c>
+      <c r="X17" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1330,9 +1548,27 @@
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
       <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-    </row>
-    <row r="19" spans="1:20">
+      <c r="T18" s="23"/>
+      <c r="U18" s="3">
+        <v>-0.03</v>
+      </c>
+      <c r="V18" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="W18" s="3">
+        <v>-0.06</v>
+      </c>
+      <c r="X18" s="3">
+        <v>-0.03</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1356,9 +1592,27 @@
       <c r="Q19" s="16"/>
       <c r="R19" s="16"/>
       <c r="S19" s="16"/>
-      <c r="T19" s="16"/>
-    </row>
-    <row r="20" spans="1:20">
+      <c r="T19" s="23"/>
+      <c r="U19" s="3">
+        <v>-0.03</v>
+      </c>
+      <c r="V19" s="3">
+        <v>-0.09</v>
+      </c>
+      <c r="W19" s="3">
+        <v>-0.05</v>
+      </c>
+      <c r="X19" s="3">
+        <v>-0.03</v>
+      </c>
+      <c r="Y19" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1403,9 +1657,9 @@
       <c r="Q20" s="16"/>
       <c r="R20" s="16"/>
       <c r="S20" s="16"/>
-      <c r="T20" s="16"/>
-    </row>
-    <row r="21" spans="1:20">
+      <c r="T20" s="23"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1453,9 +1707,27 @@
       <c r="Q21" s="16"/>
       <c r="R21" s="16"/>
       <c r="S21" s="16"/>
-      <c r="T21" s="16"/>
-    </row>
-    <row r="22" spans="1:20">
+      <c r="T21" s="23"/>
+      <c r="U21" s="3">
+        <v>-0.04</v>
+      </c>
+      <c r="V21" s="3">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="W21" s="3">
+        <v>-0.05</v>
+      </c>
+      <c r="X21" s="3">
+        <v>-0.04</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>-0.03</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1479,9 +1751,27 @@
       <c r="Q22" s="16"/>
       <c r="R22" s="16"/>
       <c r="S22" s="16"/>
-      <c r="T22" s="16"/>
-    </row>
-    <row r="23" spans="1:20">
+      <c r="T22" s="23"/>
+      <c r="U22" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="V22" s="3">
+        <v>-0.03</v>
+      </c>
+      <c r="W22" s="3">
+        <v>0</v>
+      </c>
+      <c r="X22" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1505,9 +1795,27 @@
       <c r="Q23" s="16"/>
       <c r="R23" s="16"/>
       <c r="S23" s="16"/>
-      <c r="T23" s="16"/>
-    </row>
-    <row r="24" spans="1:20">
+      <c r="T23" s="23"/>
+      <c r="U23" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="V23" s="3">
+        <v>-0.02</v>
+      </c>
+      <c r="W23" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="X23" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="Y23" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="Z23" s="3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1531,9 +1839,27 @@
       <c r="Q24" s="16"/>
       <c r="R24" s="16"/>
       <c r="S24" s="16"/>
-      <c r="T24" s="16"/>
-    </row>
-    <row r="25" spans="1:20">
+      <c r="T24" s="23"/>
+      <c r="U24" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="V24" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="W24" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="X24" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="Y24" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1578,9 +1904,9 @@
       <c r="Q25" s="16"/>
       <c r="R25" s="16"/>
       <c r="S25" s="16"/>
-      <c r="T25" s="16"/>
-    </row>
-    <row r="26" spans="1:20">
+      <c r="T25" s="23"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1616,9 +1942,9 @@
       <c r="Q26" s="16"/>
       <c r="R26" s="16"/>
       <c r="S26" s="16"/>
-      <c r="T26" s="16"/>
-    </row>
-    <row r="27" spans="1:20">
+      <c r="T26" s="23"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1654,9 +1980,9 @@
       <c r="Q27" s="16"/>
       <c r="R27" s="16"/>
       <c r="S27" s="16"/>
-      <c r="T27" s="16"/>
-    </row>
-    <row r="28" spans="1:20">
+      <c r="T27" s="23"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -1692,9 +2018,9 @@
       <c r="Q28" s="16"/>
       <c r="R28" s="16"/>
       <c r="S28" s="16"/>
-      <c r="T28" s="16"/>
-    </row>
-    <row r="29" spans="1:20">
+      <c r="T28" s="23"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -1730,9 +2056,9 @@
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
       <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
-    </row>
-    <row r="30" spans="1:20">
+      <c r="T29" s="23"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1750,14 +2076,14 @@
       <c r="Q30" s="16"/>
       <c r="R30" s="16"/>
       <c r="S30" s="16"/>
-      <c r="T30" s="16"/>
-    </row>
-    <row r="31" spans="1:20">
+      <c r="T30" s="23"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>20</v>
       </c>
       <c r="B31">
-        <v>2.6</v>
+        <v>2.48</v>
       </c>
       <c r="C31" s="2">
         <v>1.8120000000000001</v>
@@ -1788,9 +2114,27 @@
       <c r="Q31" s="16"/>
       <c r="R31" s="16"/>
       <c r="S31" s="16"/>
-      <c r="T31" s="16"/>
-    </row>
-    <row r="32" spans="1:20">
+      <c r="T31" s="23"/>
+      <c r="U31" s="17">
+        <v>1.74</v>
+      </c>
+      <c r="V31" s="17">
+        <v>1.04</v>
+      </c>
+      <c r="W31" s="17">
+        <v>1.52</v>
+      </c>
+      <c r="X31" s="17">
+        <v>1.73</v>
+      </c>
+      <c r="Y31" s="17">
+        <v>1.97</v>
+      </c>
+      <c r="Z31" s="17">
+        <v>2.4300000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1830,11 +2174,29 @@
       <c r="S32" s="18">
         <v>0.38600000000000001</v>
       </c>
-      <c r="T32" s="18">
+      <c r="T32" s="25">
         <v>0.42499999999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:20">
+      <c r="U32" s="17">
+        <v>-1.62</v>
+      </c>
+      <c r="V32" s="17">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="W32" s="17">
+        <v>-1.85</v>
+      </c>
+      <c r="X32" s="17">
+        <v>-1.62</v>
+      </c>
+      <c r="Y32" s="17">
+        <v>-1.4</v>
+      </c>
+      <c r="Z32" s="17">
+        <v>-0.93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1874,11 +2236,29 @@
       <c r="S33" s="18">
         <v>0.499</v>
       </c>
-      <c r="T33" s="18">
+      <c r="T33" s="25">
         <v>0.53800000000000003</v>
       </c>
-    </row>
-    <row r="34" spans="1:20">
+      <c r="U33" s="17">
+        <v>-0.83</v>
+      </c>
+      <c r="V33" s="17">
+        <v>-1.52</v>
+      </c>
+      <c r="W33" s="17">
+        <v>-1.06</v>
+      </c>
+      <c r="X33" s="17">
+        <v>-0.83</v>
+      </c>
+      <c r="Y33" s="17">
+        <v>-0.61</v>
+      </c>
+      <c r="Z33" s="17">
+        <v>-0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1918,11 +2298,29 @@
       <c r="S34" s="18">
         <v>0.63600000000000001</v>
       </c>
-      <c r="T34" s="18">
+      <c r="T34" s="25">
         <v>0.67500000000000004</v>
       </c>
-    </row>
-    <row r="35" spans="1:20">
+      <c r="U34" s="17">
+        <v>-0.54</v>
+      </c>
+      <c r="V34" s="17">
+        <v>-1.22</v>
+      </c>
+      <c r="W34" s="17">
+        <v>-0.77</v>
+      </c>
+      <c r="X34" s="17">
+        <v>-0.53</v>
+      </c>
+      <c r="Y34" s="17">
+        <v>-0.32</v>
+      </c>
+      <c r="Z34" s="17">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1962,11 +2360,29 @@
       <c r="S35" s="18">
         <v>1.4890000000000001</v>
       </c>
-      <c r="T35" s="18">
+      <c r="T35" s="25">
         <v>1.528</v>
       </c>
-    </row>
-    <row r="36" spans="1:20">
+      <c r="U35" s="17">
+        <v>-0.02</v>
+      </c>
+      <c r="V35" s="17">
+        <v>-0.7</v>
+      </c>
+      <c r="W35" s="17">
+        <v>-0.25</v>
+      </c>
+      <c r="X35" s="17">
+        <v>-0.01</v>
+      </c>
+      <c r="Y35" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="Z35" s="17">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2006,11 +2422,29 @@
       <c r="S36" s="18">
         <v>1.82</v>
       </c>
-      <c r="T36" s="18">
+      <c r="T36" s="25">
         <v>1.861</v>
       </c>
-    </row>
-    <row r="37" spans="1:20">
+      <c r="U36" s="17">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="V36" s="17">
+        <v>-0.39</v>
+      </c>
+      <c r="W36" s="17">
+        <v>0.06</v>
+      </c>
+      <c r="X36" s="17">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="Y36" s="17">
+        <v>0.51</v>
+      </c>
+      <c r="Z36" s="17">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -2050,11 +2484,29 @@
       <c r="S37" s="18">
         <v>2.3769999999999998</v>
       </c>
-      <c r="T37" s="18">
+      <c r="T37" s="25">
         <v>2.415</v>
       </c>
-    </row>
-    <row r="38" spans="1:20">
+      <c r="U37" s="17">
+        <v>1.06</v>
+      </c>
+      <c r="V37" s="17">
+        <v>0.37</v>
+      </c>
+      <c r="W37" s="17">
+        <v>0.83</v>
+      </c>
+      <c r="X37" s="17">
+        <v>1.07</v>
+      </c>
+      <c r="Y37" s="17">
+        <v>1.28</v>
+      </c>
+      <c r="Z37" s="17">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2094,11 +2546,29 @@
       <c r="S38" s="18">
         <v>2.9710000000000001</v>
       </c>
-      <c r="T38" s="18">
+      <c r="T38" s="25">
         <v>3.012</v>
       </c>
-    </row>
-    <row r="39" spans="1:20">
+      <c r="U38" s="17">
+        <v>1.64</v>
+      </c>
+      <c r="V38" s="17">
+        <v>0.96</v>
+      </c>
+      <c r="W38" s="17">
+        <v>1.41</v>
+      </c>
+      <c r="X38" s="17">
+        <v>1.64</v>
+      </c>
+      <c r="Y38" s="17">
+        <v>1.86</v>
+      </c>
+      <c r="Z38" s="17">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -2116,41 +2586,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Fake data with larger parameters
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="105" yWindow="0" windowWidth="25185" windowHeight="15825"/>
+    <workbookView xWindow="105" yWindow="0" windowWidth="25185" windowHeight="15825" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
-    <sheet name="meta" sheetId="2" r:id="rId2"/>
+    <sheet name="bigcoeff" sheetId="3" r:id="rId2"/>
+    <sheet name="meta" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
   <si>
     <t>Variable</t>
   </si>
@@ -187,13 +188,19 @@
   </si>
   <si>
     <t>0.9 (but the actual avg is 1.00)</t>
+  </si>
+  <si>
+    <t>Blue means the model doesn't incdue the actual value in a 50% CrI</t>
+  </si>
+  <si>
+    <t>Fake param (germdate_fakedata_bigcoeff.R)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,8 +252,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,6 +288,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,7 +348,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -356,6 +382,15 @@
     <xf numFmtId="9" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -676,11 +711,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="Y3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AG10" sqref="AG10"/>
+      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3072,55 +3107,764 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:O35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="36">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E2" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="F2" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="H2" s="38">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>1.5</v>
+      </c>
+      <c r="C3">
+        <v>1.48</v>
+      </c>
+      <c r="D3">
+        <v>1.41</v>
+      </c>
+      <c r="E3">
+        <v>1.45</v>
+      </c>
+      <c r="F3">
+        <v>1.48</v>
+      </c>
+      <c r="G3">
+        <v>1.5</v>
+      </c>
+      <c r="H3">
+        <v>1.53</v>
+      </c>
+      <c r="J3" s="21"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="20"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <v>-1.01</v>
+      </c>
+      <c r="D4">
+        <v>-1.07</v>
+      </c>
+      <c r="E4">
+        <v>-1.03</v>
+      </c>
+      <c r="F4">
+        <v>-1.01</v>
+      </c>
+      <c r="G4">
+        <v>-0.98</v>
+      </c>
+      <c r="H4">
+        <v>-0.94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2.02</v>
+      </c>
+      <c r="D5">
+        <v>1.96</v>
+      </c>
+      <c r="E5">
+        <v>1.99</v>
+      </c>
+      <c r="F5">
+        <v>2.02</v>
+      </c>
+      <c r="G5">
+        <v>2.04</v>
+      </c>
+      <c r="H5">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>1.9</v>
+      </c>
+      <c r="C6" s="40">
+        <v>1.93</v>
+      </c>
+      <c r="D6" s="40">
+        <v>1.87</v>
+      </c>
+      <c r="E6" s="40">
+        <v>1.91</v>
+      </c>
+      <c r="F6" s="40">
+        <v>1.93</v>
+      </c>
+      <c r="G6" s="40">
+        <v>1.95</v>
+      </c>
+      <c r="H6" s="40">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0.94</v>
+      </c>
+      <c r="E7">
+        <v>0.98</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1.02</v>
+      </c>
+      <c r="H7">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>-1</v>
+      </c>
+      <c r="C12" s="40">
+        <v>-0.88</v>
+      </c>
+      <c r="D12" s="40">
+        <v>-0.96</v>
+      </c>
+      <c r="E12" s="40">
+        <v>-0.91</v>
+      </c>
+      <c r="F12" s="40">
+        <v>-0.88</v>
+      </c>
+      <c r="G12" s="40">
+        <v>-0.85</v>
+      </c>
+      <c r="H12" s="40">
+        <v>-0.79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>-2</v>
+      </c>
+      <c r="C13" s="41">
+        <v>-1.99</v>
+      </c>
+      <c r="D13" s="41">
+        <v>-2.08</v>
+      </c>
+      <c r="E13" s="41">
+        <v>-2.02</v>
+      </c>
+      <c r="F13" s="41">
+        <v>-1.99</v>
+      </c>
+      <c r="G13" s="41">
+        <v>-1.96</v>
+      </c>
+      <c r="H13" s="41">
+        <v>-1.91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>-3</v>
+      </c>
+      <c r="C14">
+        <v>-2.97</v>
+      </c>
+      <c r="D14">
+        <v>-3.06</v>
+      </c>
+      <c r="E14">
+        <v>-3</v>
+      </c>
+      <c r="F14">
+        <v>-2.97</v>
+      </c>
+      <c r="G14">
+        <v>-2.94</v>
+      </c>
+      <c r="H14">
+        <v>-2.88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>-2</v>
+      </c>
+      <c r="C15">
+        <v>-1.99</v>
+      </c>
+      <c r="D15">
+        <v>-2.0699999999999998</v>
+      </c>
+      <c r="E15">
+        <v>-2.02</v>
+      </c>
+      <c r="F15">
+        <v>-1.99</v>
+      </c>
+      <c r="G15">
+        <v>-1.96</v>
+      </c>
+      <c r="H15">
+        <v>-1.91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>-1</v>
+      </c>
+      <c r="C16">
+        <v>-1.02</v>
+      </c>
+      <c r="D16">
+        <v>-1.1100000000000001</v>
+      </c>
+      <c r="E16">
+        <v>-1.05</v>
+      </c>
+      <c r="F16">
+        <v>-1.02</v>
+      </c>
+      <c r="G16">
+        <v>-0.99</v>
+      </c>
+      <c r="H16">
+        <v>-0.94</v>
+      </c>
+      <c r="I16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>-2</v>
+      </c>
+      <c r="C17">
+        <v>-2.0099999999999998</v>
+      </c>
+      <c r="D17">
+        <v>-2.09</v>
+      </c>
+      <c r="E17">
+        <v>-2.04</v>
+      </c>
+      <c r="F17">
+        <v>-2.0099999999999998</v>
+      </c>
+      <c r="G17">
+        <v>-1.98</v>
+      </c>
+      <c r="H17">
+        <v>-1.92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" s="39">
+        <v>3.11</v>
+      </c>
+      <c r="D18" s="39">
+        <v>2.99</v>
+      </c>
+      <c r="E18" s="39">
+        <v>3.07</v>
+      </c>
+      <c r="F18" s="39">
+        <v>3.11</v>
+      </c>
+      <c r="G18" s="39">
+        <v>3.15</v>
+      </c>
+      <c r="H18" s="39">
+        <v>3.22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>3.01</v>
+      </c>
+      <c r="D19">
+        <v>2.89</v>
+      </c>
+      <c r="E19">
+        <v>2.96</v>
+      </c>
+      <c r="F19">
+        <v>3.01</v>
+      </c>
+      <c r="G19">
+        <v>3.05</v>
+      </c>
+      <c r="H19">
+        <v>3.13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" s="39">
+        <v>2.94</v>
+      </c>
+      <c r="D20" s="39">
+        <v>2.82</v>
+      </c>
+      <c r="E20" s="39">
+        <v>2.9</v>
+      </c>
+      <c r="F20" s="39">
+        <v>2.94</v>
+      </c>
+      <c r="G20" s="39">
+        <v>2.98</v>
+      </c>
+      <c r="H20" s="39">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27">
+        <v>2.48</v>
+      </c>
+      <c r="C27">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="D27">
+        <v>1.8</v>
+      </c>
+      <c r="E27">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="F27">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="G27">
+        <v>2.7</v>
+      </c>
+      <c r="H27">
+        <v>3.19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>-1.5</v>
+      </c>
+      <c r="C28">
+        <v>-1.52</v>
+      </c>
+      <c r="D28">
+        <v>-2.23</v>
+      </c>
+      <c r="E28">
+        <v>-1.73</v>
+      </c>
+      <c r="F28">
+        <v>-1.52</v>
+      </c>
+      <c r="G28">
+        <v>-1.29</v>
+      </c>
+      <c r="H28">
+        <v>-0.84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <v>-1</v>
+      </c>
+      <c r="C29">
+        <v>-0.91</v>
+      </c>
+      <c r="D29">
+        <v>-1.62</v>
+      </c>
+      <c r="E29">
+        <v>-1.1299999999999999</v>
+      </c>
+      <c r="F29">
+        <v>-0.91</v>
+      </c>
+      <c r="G29">
+        <v>-0.69</v>
+      </c>
+      <c r="H29">
+        <v>-0.23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>-0.5</v>
+      </c>
+      <c r="C30">
+        <v>-0.65</v>
+      </c>
+      <c r="D30">
+        <v>-1.36</v>
+      </c>
+      <c r="E30">
+        <v>-0.86</v>
+      </c>
+      <c r="F30">
+        <v>-0.65</v>
+      </c>
+      <c r="G30">
+        <v>-0.42</v>
+      </c>
+      <c r="H30">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>-0.03</v>
+      </c>
+      <c r="D31">
+        <v>-0.74</v>
+      </c>
+      <c r="E31">
+        <v>-0.24</v>
+      </c>
+      <c r="F31">
+        <v>-0.02</v>
+      </c>
+      <c r="G31">
+        <v>0.2</v>
+      </c>
+      <c r="H31">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32">
+        <v>0.5</v>
+      </c>
+      <c r="C32">
+        <v>0.51</v>
+      </c>
+      <c r="D32">
+        <v>-0.2</v>
+      </c>
+      <c r="E32">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F32">
+        <v>0.51</v>
+      </c>
+      <c r="G32">
+        <v>0.73</v>
+      </c>
+      <c r="H32">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>1.02</v>
+      </c>
+      <c r="D33">
+        <v>0.32</v>
+      </c>
+      <c r="E33">
+        <v>0.81</v>
+      </c>
+      <c r="F33">
+        <v>1.03</v>
+      </c>
+      <c r="G33">
+        <v>1.25</v>
+      </c>
+      <c r="H33">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>1.5</v>
+      </c>
+      <c r="C34">
+        <v>1.47</v>
+      </c>
+      <c r="D34">
+        <v>0.76</v>
+      </c>
+      <c r="E34">
+        <v>1.26</v>
+      </c>
+      <c r="F34">
+        <v>1.47</v>
+      </c>
+      <c r="G34">
+        <v>1.69</v>
+      </c>
+      <c r="H34">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>50</v>
       </c>

</xml_diff>